<commit_message>
new random weight points
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -21,6 +21,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -156,7 +160,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="power"/>
+            <c:trendlineType val="exp"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -218,15 +222,6 @@
                 <c:pt idx="6">
                   <c:v>8192.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>16384.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>32768.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>65536.0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -237,34 +232,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.15368</c:v>
+                  <c:v>1.30413</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.18902</c:v>
+                  <c:v>1.34523</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.17627</c:v>
+                  <c:v>1.1829</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.21929</c:v>
+                  <c:v>2.21169</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.18742</c:v>
+                  <c:v>1.23711</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.20502</c:v>
+                  <c:v>1.19623</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.20758</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.20822</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.20331</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.20321</c:v>
+                  <c:v>1.20377</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7643,15 +7629,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>164846</xdr:colOff>
+      <xdr:colOff>20528</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>43295</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>574524</xdr:colOff>
+      <xdr:colOff>430206</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>106809</xdr:rowOff>
+      <xdr:rowOff>150104</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8149,7 +8135,7 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="88" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8159,7 +8145,7 @@
         <v>128</v>
       </c>
       <c r="B1">
-        <v>1.15368</v>
+        <v>1.30413</v>
       </c>
       <c r="K1">
         <v>10</v>
@@ -8173,7 +8159,7 @@
         <v>256</v>
       </c>
       <c r="B2">
-        <v>1.18902</v>
+        <v>1.3452299999999999</v>
       </c>
       <c r="K2">
         <v>20</v>
@@ -8187,7 +8173,7 @@
         <v>512</v>
       </c>
       <c r="B3">
-        <v>1.1762699999999999</v>
+        <v>1.1829000000000001</v>
       </c>
       <c r="K3">
         <v>25</v>
@@ -8201,7 +8187,7 @@
         <v>1024</v>
       </c>
       <c r="B4">
-        <v>1.21929</v>
+        <v>2.2116899999999999</v>
       </c>
       <c r="K4">
         <v>40</v>
@@ -8215,7 +8201,7 @@
         <v>2048</v>
       </c>
       <c r="B5">
-        <v>1.1874199999999999</v>
+        <v>1.2371099999999999</v>
       </c>
       <c r="K5">
         <v>50</v>
@@ -8229,7 +8215,7 @@
         <v>4096</v>
       </c>
       <c r="B6">
-        <v>1.20502</v>
+        <v>1.1962299999999999</v>
       </c>
       <c r="K6">
         <v>75</v>
@@ -8243,7 +8229,7 @@
         <v>8192</v>
       </c>
       <c r="B7">
-        <v>1.2075800000000001</v>
+        <v>1.20377</v>
       </c>
       <c r="K7">
         <v>100</v>
@@ -8253,12 +8239,6 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>16384</v>
-      </c>
-      <c r="B8">
-        <v>1.2082200000000001</v>
-      </c>
       <c r="K8">
         <v>200</v>
       </c>
@@ -8267,12 +8247,6 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>32768</v>
-      </c>
-      <c r="B9">
-        <v>1.2033100000000001</v>
-      </c>
       <c r="K9">
         <v>250</v>
       </c>
@@ -8281,12 +8255,6 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>65536</v>
-      </c>
-      <c r="B10">
-        <v>1.2032099999999999</v>
-      </c>
       <c r="K10">
         <v>400</v>
       </c>

</xml_diff>

<commit_message>
correct random graph data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -160,7 +160,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="exp"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -241,7 +241,7 @@
                   <c:v>1.1829</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.21169</c:v>
+                  <c:v>1.21169</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.23711</c:v>
@@ -8135,7 +8135,7 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="88" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8187,7 +8187,7 @@
         <v>1024</v>
       </c>
       <c r="B4">
-        <v>2.2116899999999999</v>
+        <v>1.2116899999999999</v>
       </c>
       <c r="K4">
         <v>40</v>

</xml_diff>